<commit_message>
Lost of code changes
Lost of code changes
</commit_message>
<xml_diff>
--- a/Netbeans Project File/Demonstration Parade Route/Input Route Data Template.xlsx
+++ b/Netbeans Project File/Demonstration Parade Route/Input Route Data Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\Data-Structure-Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\Data-Structure-Design\Netbeans Project File\Demonstration Parade Route\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4D44DF-704E-4614-8A11-69AED941CE3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FCB2C6-82FB-4B5B-87E2-5922A712F1A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8970" xr2:uid="{B96E8E76-8475-4F7C-8615-E3CDEC40FC00}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>시위대명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -44,27 +44,83 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>인원</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>14:00~16:00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>남대문,서울역,남대문,대한문</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>…</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>중부, 종로, 남대문 관내 행진 교차로 Template</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>민주노총</t>
+    <t>새한국</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>청계광장→세종→세문관→광화문→동십자→안국→인사동→종로2→종로1→서린→세종→청계광장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구명총</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:40~17:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:30~17:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태극기국민평의회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한은→눈스퀘어→을지1→광교→종로1→서린→세종</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>석방운동본부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:30~19:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서울역→남대문→한은→눈스퀘어→을지1→광교→종로1→서린→세종→세문관↔광화문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태극기행동본부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:20~18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세종→세문관→광화문→동십자→안국→인사동→종로2→종로1→서린→세종</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태극기국민운동본부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:30~18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대한문→환구단→개풍→을지1→눈스퀘어→한은→남대문→태평→대한문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신고 인원(명)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.02.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세종→서린→종로1→종로2→종로3→종로2→종로1→서린→세종</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -72,7 +128,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +162,15 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -115,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -163,13 +228,24 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -181,7 +257,9 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -190,35 +268,44 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -535,90 +622,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F354919E-7C38-4968-8A20-CB1CE7FDA2C4}">
-  <dimension ref="B1:I6"/>
+  <dimension ref="B1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.875" customWidth="1"/>
-    <col min="3" max="3" width="11.25" customWidth="1"/>
-    <col min="4" max="4" width="27.875" customWidth="1"/>
-    <col min="7" max="7" width="11.875" customWidth="1"/>
-    <col min="8" max="8" width="25.375" customWidth="1"/>
+    <col min="1" max="1" width="2.875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="86.25" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="2:9" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+    <row r="1" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="2:6" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7">
+        <v>300</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="2:9" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="E6" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7">
+        <v>100</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="3">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>6</v>
+      <c r="E7" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7">
+        <v>100</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7">
+        <v>3000</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7">
+        <v>300</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="7">
+        <v>600</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B4:E4"/>
     <mergeCell ref="B2:E2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>